<commit_message>
Monte Carlo module added to PyDSS
</commit_message>
<xml_diff>
--- a/ProjectFiles/IEEE13/PyDSS Settings/Socket/pyControllerList/Socket Controller.xlsx
+++ b/ProjectFiles/IEEE13/PyDSS Settings/Socket/pyControllerList/Socket Controller.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0002A265-F411-4037-8402-ECA2CAA275B3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>None</t>
   </si>
@@ -90,6 +91,12 @@
   </si>
   <si>
     <t>Multiple of 2</t>
+  </si>
+  <si>
+    <t>Modbus</t>
+  </si>
+  <si>
+    <t>DNP3</t>
   </si>
 </sst>
 </file>
@@ -766,22 +773,22 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="10" t="s">
         <v>19</v>
@@ -799,7 +806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -825,7 +832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -862,12 +869,18 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{55729431-ED51-49A5-897E-D01AFD1BB9B0}">
           <x14:formula1>
             <xm:f>Settings!$A$3:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:E1048576 E3</xm:sqref>
+          <xm:sqref>E4:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{57FA777C-D898-424C-9B56-9D6E46B867CA}">
+          <x14:formula1>
+            <xm:f>Settings!$A$3:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -877,25 +890,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F16498-3560-4815-B70E-DD12ED8C6DF7}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -903,7 +918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -911,17 +926,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>